<commit_message>
First working model run
</commit_message>
<xml_diff>
--- a/virginia/data/scenarios.xlsx
+++ b/virginia/data/scenarios.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10615"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{466138AF-0862-E943-BCBA-56328BFFA035}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D7CBDC5-6105-7E47-93DA-C664B7F16BF9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="23260" windowHeight="12580" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SolverSettings" sheetId="2" r:id="rId1"/>
@@ -522,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:G10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -534,7 +534,7 @@
     <col min="2" max="3" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -542,7 +542,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -550,39 +550,59 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>24</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>25</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>26</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>39</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>41</v>
       </c>
@@ -590,7 +610,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -598,7 +618,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -606,7 +626,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>59</v>
       </c>
@@ -625,7 +645,7 @@
   <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C1" sqref="C1:C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -860,7 +880,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C1" sqref="C1:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -957,8 +977,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>